<commit_message>
Start work on the form
</commit_message>
<xml_diff>
--- a/MUSCShieldForm.xlsx
+++ b/MUSCShieldForm.xlsx
@@ -9,14 +9,15 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="20490" windowHeight="9630" activeTab="1"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="20490" windowHeight="9630"/>
   </bookViews>
   <sheets>
-    <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
-    <sheet name="PET" sheetId="2" r:id="rId2"/>
+    <sheet name="Sheet2" sheetId="3" r:id="rId1"/>
+    <sheet name="Sheet1" sheetId="1" r:id="rId2"/>
+    <sheet name="PET" sheetId="2" r:id="rId3"/>
   </sheets>
   <externalReferences>
-    <externalReference r:id="rId3"/>
+    <externalReference r:id="rId4"/>
   </externalReferences>
   <definedNames>
     <definedName name="alpha">#REF!</definedName>
@@ -24,7 +25,6 @@
     <definedName name="gamma">#REF!</definedName>
     <definedName name="minimum_Pb">[1]Table!$AG$6:$AG$41</definedName>
     <definedName name="mm_value">[1]Table!$AE$6:$AE$41</definedName>
-    <definedName name="_xlnm.Print_Area" localSheetId="0">Sheet1!$A$1:$I$22</definedName>
     <definedName name="RefDist">[1]ShieldEvaluation!$F$16</definedName>
     <definedName name="RefExp">[1]ShieldEvaluation!$G$16</definedName>
     <definedName name="RefkV">[1]ShieldEvaluation!$C$16</definedName>
@@ -39,8 +39,141 @@
 </workbook>
 </file>
 
+<file path=xl/comments1.xml><?xml version="1.0" encoding="utf-8"?>
+<comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <authors>
+    <author>Eugene Mah</author>
+  </authors>
+  <commentList>
+    <comment ref="K29" authorId="0" shapeId="0">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <charset val="1"/>
+          </rPr>
+          <t>Eugene Mah:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <charset val="1"/>
+          </rPr>
+          <t xml:space="preserve">
+Dose limits per NCRP 116 recommendations.</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="D30" authorId="0" shapeId="0">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <charset val="1"/>
+          </rPr>
+          <t>Eugene Mah:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <charset val="1"/>
+          </rPr>
+          <t xml:space="preserve">
+Distance from primary beam (m)</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="H30" authorId="0" shapeId="0">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <charset val="1"/>
+          </rPr>
+          <t>Eugene Mah:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <charset val="1"/>
+          </rPr>
+          <t xml:space="preserve">
+Use factor</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="I30" authorId="0" shapeId="0">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <charset val="1"/>
+          </rPr>
+          <t>Eugene Mah:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <charset val="1"/>
+          </rPr>
+          <t xml:space="preserve">
+Occupancy factor</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="J30" authorId="0" shapeId="0">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <charset val="1"/>
+          </rPr>
+          <t>Eugene Mah:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <charset val="1"/>
+          </rPr>
+          <t xml:space="preserve">
+Type of area
+U - Uncontrolled
+C - Controlled
+C if blank</t>
+        </r>
+      </text>
+    </comment>
+  </commentList>
+</comments>
+</file>
+
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="60" uniqueCount="37">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="112" uniqueCount="66">
   <si>
     <t>P</t>
   </si>
@@ -151,13 +284,105 @@
   </si>
   <si>
     <t>Wood</t>
+  </si>
+  <si>
+    <t>Medical University of South Carolina</t>
+  </si>
+  <si>
+    <t>Charleston, South Carolina</t>
+  </si>
+  <si>
+    <t>Radiation Shielding</t>
+  </si>
+  <si>
+    <t>Location Information</t>
+  </si>
+  <si>
+    <t>Location</t>
+  </si>
+  <si>
+    <t>Facility:</t>
+  </si>
+  <si>
+    <t>Department:</t>
+  </si>
+  <si>
+    <t>Area/Division</t>
+  </si>
+  <si>
+    <t>Workload Information</t>
+  </si>
+  <si>
+    <t># Patients/week:</t>
+  </si>
+  <si>
+    <t>Date:</t>
+  </si>
+  <si>
+    <t>Views/patient:</t>
+  </si>
+  <si>
+    <t>Weekly workload (mA-min):</t>
+  </si>
+  <si>
+    <t>Workload/patient (mA-min/pt):</t>
+  </si>
+  <si>
+    <t>Type of Room:</t>
+  </si>
+  <si>
+    <t>Performed by:</t>
+  </si>
+  <si>
+    <t>Unshielded primary air kerma per patient (Kp)</t>
+  </si>
+  <si>
+    <t>Primary field size (cm^2):</t>
+  </si>
+  <si>
+    <t>Unshielded secondary air kerma per patient (Ksec)</t>
+  </si>
+  <si>
+    <t>D(pri)</t>
+  </si>
+  <si>
+    <t>All distances in meters</t>
+  </si>
+  <si>
+    <t>Fit parameters</t>
+  </si>
+  <si>
+    <t>Conversion Assistance</t>
+  </si>
+  <si>
+    <t>Feet</t>
+  </si>
+  <si>
+    <t>Meter</t>
+  </si>
+  <si>
+    <t>inch</t>
+  </si>
+  <si>
+    <t>mm</t>
+  </si>
+  <si>
+    <t>Transmission</t>
+  </si>
+  <si>
+    <t>B(x)</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="3" x14ac:knownFonts="1">
+  <numFmts count="3">
+    <numFmt numFmtId="164" formatCode="0.0"/>
+    <numFmt numFmtId="165" formatCode="0.000E+00"/>
+    <numFmt numFmtId="166" formatCode="0.000"/>
+  </numFmts>
+  <fonts count="8" x14ac:knownFonts="1">
     <font>
       <sz val="10"/>
       <name val="Times New Roman"/>
@@ -175,16 +400,53 @@
       <name val="Times New Roman"/>
       <family val="1"/>
     </font>
+    <font>
+      <sz val="10"/>
+      <name val="Times New Roman"/>
+      <family val="1"/>
+    </font>
+    <font>
+      <b/>
+      <i/>
+      <sz val="14"/>
+      <name val="Monotype Corsiva"/>
+      <family val="4"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="14"/>
+      <name val="Times New Roman"/>
+      <family val="1"/>
+    </font>
+    <font>
+      <sz val="9"/>
+      <color indexed="81"/>
+      <name val="Tahoma"/>
+      <charset val="1"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="9"/>
+      <color indexed="81"/>
+      <name val="Tahoma"/>
+      <charset val="1"/>
+    </font>
   </fonts>
-  <fills count="2">
+  <fills count="3">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor indexed="26"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="2">
+  <borders count="4">
     <border>
       <left/>
       <right/>
@@ -203,13 +465,33 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top/>
+      <bottom style="dotted">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0">
       <alignment horizontal="center"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="6">
+  <cellXfs count="17">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
       <alignment horizontal="center"/>
     </xf>
@@ -227,6 +509,41 @@
     </xf>
     <xf numFmtId="2" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1">
       <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="3" fillId="2" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyBorder="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="166" fontId="3" fillId="2" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center"/>
+      <protection locked="0"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -549,13 +866,16 @@
       <sheetData sheetId="1"/>
       <sheetData sheetId="2">
         <row r="16">
+          <cell r="C16"/>
+          <cell r="F16"/>
+          <cell r="G16"/>
           <cell r="H16" t="str">
             <v/>
           </cell>
         </row>
       </sheetData>
-      <sheetData sheetId="3" refreshError="1"/>
-      <sheetData sheetId="4" refreshError="1"/>
+      <sheetData sheetId="3"/>
+      <sheetData sheetId="4"/>
     </sheetDataSet>
   </externalBook>
 </externalLink>
@@ -823,10 +1143,270 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="B2:R30"/>
+  <sheetViews>
+    <sheetView tabSelected="1" topLeftCell="A13" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="A31" sqref="A31"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="11.25" customHeight="1" x14ac:dyDescent="0.2"/>
+  <sheetData>
+    <row r="2" spans="2:18" ht="11.25" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="G2" s="6" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="3" spans="2:18" ht="11.25" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="G3" s="6" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="4" spans="2:18" ht="11.25" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="G4" s="7"/>
+    </row>
+    <row r="5" spans="2:18" ht="11.25" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="G5" s="8" t="s">
+        <v>39</v>
+      </c>
+      <c r="O5" s="12" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="6" spans="2:18" ht="11.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="O6" s="13" t="s">
+        <v>60</v>
+      </c>
+      <c r="P6" s="13" t="s">
+        <v>61</v>
+      </c>
+      <c r="Q6" s="13" t="s">
+        <v>61</v>
+      </c>
+      <c r="R6" s="13" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="7" spans="2:18" ht="11.25" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="G7" s="8" t="s">
+        <v>40</v>
+      </c>
+      <c r="O7" s="14"/>
+      <c r="P7" s="4">
+        <f>O7*12*0.0254</f>
+        <v>0</v>
+      </c>
+      <c r="Q7" s="14"/>
+      <c r="R7" s="4">
+        <f>Q7*100/2.54/12</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="8" spans="2:18" ht="11.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="O8" s="13" t="s">
+        <v>62</v>
+      </c>
+      <c r="P8" s="13" t="s">
+        <v>63</v>
+      </c>
+      <c r="Q8" s="15" t="s">
+        <v>63</v>
+      </c>
+      <c r="R8" s="15" t="s">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="9" spans="2:18" ht="11.25" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="B9" t="s">
+        <v>41</v>
+      </c>
+      <c r="J9" t="s">
+        <v>45</v>
+      </c>
+      <c r="O9" s="16"/>
+      <c r="P9" s="4">
+        <f>O9*25.4</f>
+        <v>0</v>
+      </c>
+      <c r="Q9" s="16"/>
+      <c r="R9" s="4">
+        <f>Q9/25.4</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="10" spans="2:18" ht="11.25" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="C10" s="9" t="s">
+        <v>47</v>
+      </c>
+      <c r="J10" s="9" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="11" spans="2:18" ht="11.25" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="C11" s="9" t="s">
+        <v>42</v>
+      </c>
+      <c r="J11" s="9" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="12" spans="2:18" ht="11.25" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="C12" s="9" t="s">
+        <v>43</v>
+      </c>
+      <c r="J12" s="9" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="13" spans="2:18" ht="11.25" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="C13" s="9" t="s">
+        <v>44</v>
+      </c>
+      <c r="J13" s="9" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="14" spans="2:18" ht="11.25" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="C14" s="9" t="s">
+        <v>51</v>
+      </c>
+      <c r="J14" s="9" t="s">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="15" spans="2:18" ht="11.25" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="C15" s="9" t="s">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="17" spans="3:12" ht="11.25" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="D17" s="10" t="s">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="18" spans="3:12" ht="11.25" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="D18" s="10" t="s">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="20" spans="3:12" ht="11.25" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="D20" s="10" t="s">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="21" spans="3:12" ht="11.25" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="D21" t="s">
+        <v>21</v>
+      </c>
+      <c r="E21" s="2" t="s">
+        <v>22</v>
+      </c>
+      <c r="F21" s="2" t="s">
+        <v>23</v>
+      </c>
+      <c r="G21" s="2" t="s">
+        <v>24</v>
+      </c>
+      <c r="H21" s="2" t="str">
+        <f>E21&amp;G21</f>
+        <v>ag</v>
+      </c>
+      <c r="I21" s="2" t="str">
+        <f>F21&amp;"/"&amp;E21</f>
+        <v>b/a</v>
+      </c>
+    </row>
+    <row r="22" spans="3:12" ht="11.25" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="D22" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="23" spans="3:12" ht="11.25" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="D23" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="24" spans="3:12" ht="11.25" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="D24" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="25" spans="3:12" ht="11.25" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="D25" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="26" spans="3:12" ht="11.25" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="D26" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="27" spans="3:12" ht="11.25" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="D27" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="29" spans="3:12" ht="11.25" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="D29" s="11" t="s">
+        <v>57</v>
+      </c>
+      <c r="E29" s="11"/>
+      <c r="F29" s="11"/>
+      <c r="G29" s="11"/>
+      <c r="K29" t="s">
+        <v>0</v>
+      </c>
+      <c r="L29" t="s">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="30" spans="3:12" ht="11.25" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="C30" t="s">
+        <v>3</v>
+      </c>
+      <c r="D30" t="s">
+        <v>56</v>
+      </c>
+      <c r="E30" t="s">
+        <v>4</v>
+      </c>
+      <c r="F30" t="s">
+        <v>5</v>
+      </c>
+      <c r="G30" t="s">
+        <v>6</v>
+      </c>
+      <c r="H30" t="s">
+        <v>14</v>
+      </c>
+      <c r="I30" t="s">
+        <v>7</v>
+      </c>
+      <c r="J30" t="s">
+        <v>8</v>
+      </c>
+      <c r="K30" t="s">
+        <v>9</v>
+      </c>
+      <c r="L30" t="s">
+        <v>65</v>
+      </c>
+    </row>
+  </sheetData>
+  <mergeCells count="1">
+    <mergeCell ref="D29:G29"/>
+  </mergeCells>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="landscape" horizontalDpi="1200" verticalDpi="1200" r:id="rId1"/>
+  <legacyDrawing r:id="rId2"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:S22"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView zoomScaleNormal="100" workbookViewId="0">
       <selection activeCell="I3" sqref="I3"/>
     </sheetView>
   </sheetViews>
@@ -1572,15 +2152,15 @@
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" horizontalDpi="1200" verticalDpi="1200" r:id="rId1"/>
+  <pageSetup orientation="landscape" horizontalDpi="1200" verticalDpi="1200" r:id="rId1"/>
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
   <sheetData/>

</xml_diff>